<commit_message>
Excel fixed with ignoreDate
</commit_message>
<xml_diff>
--- a/public/downloads/Template Files/Accounts List Report Result.xlsx
+++ b/public/downloads/Template Files/Accounts List Report Result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RMG\Documents\Task\1-26~Excel Link\Template Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153BE5AE-D0B6-4297-B18C-94C48F05C19B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF625A1-B2AF-4B42-BFB0-CC4986BF4B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29010" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2753,20 +2753,20 @@
   <dimension ref="A1:J194"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>

</xml_diff>